<commit_message>
harmonized similar tags to be the same
</commit_message>
<xml_diff>
--- a/templates/community/CMML/MTH00029-swate-template.xlsx
+++ b/templates/community/CMML/MTH00029-swate-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dominikbrilhaus/github/nfdi4plants/Swate-templates/templates/community/CMML/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stella Eggels\Documents\GitHub\Swate-templates\templates\community\CMML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B73050D9-67BA-FF44-9931-58BE6AA839C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8E01CCB-8299-4BFB-9CB7-B6C255F0BC3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23860" yWindow="-21100" windowWidth="34220" windowHeight="19740" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MTH00029" sheetId="3" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="130">
   <si>
     <t>Source Name</t>
   </si>
@@ -238,9 +238,6 @@
     <t>Mass Spectrometry</t>
   </si>
   <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C17156</t>
-  </si>
-  <si>
     <t>Protocol Type</t>
   </si>
   <si>
@@ -419,6 +416,15 @@
   </si>
   <si>
     <t>annotationTableWonderfulBear2</t>
+  </si>
+  <si>
+    <t>NCIT:C17156</t>
+  </si>
+  <si>
+    <t>assay</t>
+  </si>
+  <si>
+    <t>OBI:0000070</t>
   </si>
 </sst>
 </file>
@@ -601,8 +607,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 3" xfId="1" xr:uid="{9AC74787-D67A-4B33-A1D2-9A84BA6D8808}"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="53">
     <dxf>
@@ -778,10 +784,7 @@
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <person displayName="Oliver Maus" id="{2B518007-AAA5-437D-AD4B-771F37659DA1}" userId="Oliver Maus" providerId="None"/>
-  <person displayName="Kevin F" id="{CF57BF67-24C4-49D6-8AA6-F7F74FCD767F}" userId="b000b0ea35d13fa4" providerId="Windows Live"/>
-</personList>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1160,60 +1163,60 @@
       <selection activeCell="AZ2" sqref="AZ2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.33203125" style="6" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30" style="6" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="38.33203125" style="6" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="35" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="36.1640625" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="33.1640625" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="33.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="36.1640625" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="36.109375" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="33.109375" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="33.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="36.109375" hidden="1" customWidth="1"/>
     <col min="11" max="11" width="26.33203125" hidden="1" customWidth="1"/>
     <col min="12" max="12" width="26.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="36.1640625" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="36.109375" hidden="1" customWidth="1"/>
     <col min="14" max="14" width="27.6640625" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="36.5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="36.1640625" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="36.44140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="36.109375" hidden="1" customWidth="1"/>
     <col min="17" max="17" width="41.33203125" hidden="1" customWidth="1"/>
     <col min="18" max="18" width="41.33203125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="36.1640625" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="36.109375" hidden="1" customWidth="1"/>
     <col min="20" max="20" width="42.33203125" hidden="1" customWidth="1"/>
     <col min="21" max="21" width="42.33203125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="36.1640625" hidden="1" customWidth="1"/>
-    <col min="23" max="23" width="36.83203125" hidden="1" customWidth="1"/>
-    <col min="24" max="24" width="36.83203125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="36.1640625" hidden="1" customWidth="1"/>
+    <col min="22" max="22" width="36.109375" hidden="1" customWidth="1"/>
+    <col min="23" max="23" width="36.77734375" hidden="1" customWidth="1"/>
+    <col min="24" max="24" width="36.77734375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="36.109375" hidden="1" customWidth="1"/>
     <col min="26" max="26" width="38.33203125" hidden="1" customWidth="1"/>
     <col min="27" max="27" width="38.33203125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="36.1640625" hidden="1" customWidth="1"/>
-    <col min="29" max="29" width="24.1640625" hidden="1" customWidth="1"/>
-    <col min="30" max="30" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="36.109375" hidden="1" customWidth="1"/>
+    <col min="29" max="29" width="24.109375" hidden="1" customWidth="1"/>
+    <col min="30" max="30" width="24.109375" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="24" hidden="1" customWidth="1"/>
-    <col min="32" max="32" width="40.5" style="7" hidden="1" customWidth="1"/>
-    <col min="33" max="33" width="40.5" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="40.44140625" style="7" hidden="1" customWidth="1"/>
+    <col min="33" max="33" width="40.44140625" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="30" hidden="1" customWidth="1"/>
-    <col min="35" max="35" width="36.1640625" hidden="1" customWidth="1"/>
+    <col min="35" max="35" width="36.109375" hidden="1" customWidth="1"/>
     <col min="36" max="36" width="39" hidden="1" customWidth="1"/>
     <col min="37" max="37" width="39" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="36.1640625" hidden="1" customWidth="1"/>
-    <col min="39" max="39" width="33.5" hidden="1" customWidth="1"/>
+    <col min="38" max="38" width="36.109375" hidden="1" customWidth="1"/>
+    <col min="39" max="39" width="33.44140625" hidden="1" customWidth="1"/>
     <col min="40" max="40" width="77" bestFit="1" customWidth="1"/>
     <col min="41" max="41" width="30" hidden="1" customWidth="1"/>
-    <col min="42" max="42" width="0.1640625" hidden="1" customWidth="1"/>
+    <col min="42" max="42" width="0.109375" hidden="1" customWidth="1"/>
     <col min="43" max="43" width="23.33203125" bestFit="1" customWidth="1"/>
     <col min="44" max="44" width="27" style="5" hidden="1" customWidth="1"/>
     <col min="45" max="45" width="32.6640625" hidden="1" customWidth="1"/>
     <col min="46" max="46" width="32.6640625" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="36.83203125" style="5" hidden="1" customWidth="1"/>
-    <col min="48" max="48" width="32.83203125" hidden="1" customWidth="1"/>
-    <col min="49" max="49" width="32.83203125" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="36.77734375" style="5" hidden="1" customWidth="1"/>
+    <col min="48" max="48" width="32.77734375" hidden="1" customWidth="1"/>
+    <col min="49" max="49" width="32.77734375" bestFit="1" customWidth="1"/>
     <col min="50" max="50" width="37" hidden="1" customWidth="1"/>
-    <col min="51" max="51" width="28.83203125" hidden="1" customWidth="1"/>
-    <col min="52" max="52" width="28.83203125" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="28.77734375" hidden="1" customWidth="1"/>
+    <col min="52" max="52" width="28.77734375" bestFit="1" customWidth="1"/>
     <col min="53" max="53" width="31" hidden="1" customWidth="1"/>
     <col min="54" max="54" width="25.33203125" hidden="1" customWidth="1"/>
     <col min="55" max="55" width="25.33203125" bestFit="1" customWidth="1"/>
@@ -1221,142 +1224,142 @@
     <col min="57" max="57" width="28" hidden="1" customWidth="1"/>
     <col min="58" max="58" width="28" bestFit="1" customWidth="1"/>
     <col min="59" max="59" width="31.6640625" hidden="1" customWidth="1"/>
-    <col min="60" max="60" width="24.5" hidden="1" customWidth="1"/>
-    <col min="61" max="61" width="24.5" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="26.83203125" hidden="1" customWidth="1"/>
+    <col min="60" max="60" width="24.44140625" hidden="1" customWidth="1"/>
+    <col min="61" max="61" width="24.44140625" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="26.77734375" hidden="1" customWidth="1"/>
     <col min="63" max="63" width="34.6640625" hidden="1" customWidth="1"/>
     <col min="64" max="64" width="34.6640625" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="38.5" hidden="1" customWidth="1"/>
-    <col min="66" max="66" width="14.1640625" hidden="1" customWidth="1"/>
-    <col min="67" max="67" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="38.44140625" hidden="1" customWidth="1"/>
+    <col min="66" max="66" width="14.109375" hidden="1" customWidth="1"/>
+    <col min="67" max="67" width="14.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" t="s">
         <v>68</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>69</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>119</v>
+      </c>
+      <c r="F1" t="s">
         <v>70</v>
       </c>
-      <c r="E1" t="s">
-        <v>120</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>71</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>72</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>73</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>74</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>75</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>76</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>77</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>78</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>79</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>80</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>81</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
+        <v>113</v>
+      </c>
+      <c r="S1" t="s">
         <v>82</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
+        <v>83</v>
+      </c>
+      <c r="U1" t="s">
         <v>114</v>
       </c>
-      <c r="S1" t="s">
-        <v>83</v>
-      </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>84</v>
       </c>
-      <c r="U1" t="s">
-        <v>115</v>
-      </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>85</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>86</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>87</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>88</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>89</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>90</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>91</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>92</v>
       </c>
       <c r="AD1" t="s">
         <v>2</v>
       </c>
       <c r="AE1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AF1" t="s">
         <v>93</v>
       </c>
-      <c r="AF1" t="s">
-        <v>94</v>
-      </c>
       <c r="AG1" t="s">
+        <v>115</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>103</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>107</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>108</v>
+      </c>
+      <c r="AK1" t="s">
         <v>116</v>
       </c>
-      <c r="AH1" t="s">
-        <v>104</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>108</v>
-      </c>
-      <c r="AJ1" t="s">
+      <c r="AL1" t="s">
         <v>109</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AM1" t="s">
+        <v>110</v>
+      </c>
+      <c r="AN1" t="s">
         <v>117</v>
       </c>
-      <c r="AL1" t="s">
-        <v>110</v>
-      </c>
-      <c r="AM1" t="s">
+      <c r="AO1" t="s">
         <v>111</v>
       </c>
-      <c r="AN1" t="s">
-        <v>118</v>
-      </c>
-      <c r="AO1" t="s">
+      <c r="AP1" t="s">
         <v>112</v>
-      </c>
-      <c r="AP1" t="s">
-        <v>113</v>
       </c>
       <c r="AQ1" t="s">
         <v>3</v>
@@ -1386,13 +1389,13 @@
         <v>11</v>
       </c>
       <c r="AZ1" t="s">
+        <v>94</v>
+      </c>
+      <c r="BA1" t="s">
         <v>95</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BB1" t="s">
         <v>96</v>
-      </c>
-      <c r="BB1" t="s">
-        <v>97</v>
       </c>
       <c r="BC1" t="s">
         <v>12</v>
@@ -1434,7 +1437,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:67" x14ac:dyDescent="0.3">
       <c r="B2" s="6" t="s">
         <v>64</v>
       </c>
@@ -1445,7 +1448,7 @@
         <v>65</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G2" t="s">
         <v>54</v>
@@ -1475,43 +1478,43 @@
         <v>54</v>
       </c>
       <c r="R2" t="s">
+        <v>120</v>
+      </c>
+      <c r="S2" t="s">
+        <v>54</v>
+      </c>
+      <c r="T2" t="s">
+        <v>54</v>
+      </c>
+      <c r="U2" t="s">
+        <v>100</v>
+      </c>
+      <c r="V2" t="s">
+        <v>54</v>
+      </c>
+      <c r="W2" t="s">
+        <v>54</v>
+      </c>
+      <c r="X2" t="s">
+        <v>101</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA2" t="s">
         <v>121</v>
       </c>
-      <c r="S2" t="s">
-        <v>54</v>
-      </c>
-      <c r="T2" t="s">
-        <v>54</v>
-      </c>
-      <c r="U2" t="s">
-        <v>101</v>
-      </c>
-      <c r="V2" t="s">
-        <v>54</v>
-      </c>
-      <c r="W2" t="s">
-        <v>54</v>
-      </c>
-      <c r="X2" t="s">
+      <c r="AB2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AD2" t="s">
         <v>102</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>54</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>54</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>122</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>54</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>54</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>103</v>
       </c>
       <c r="AE2" t="s">
         <v>54</v>
@@ -1523,16 +1526,16 @@
         <v>1</v>
       </c>
       <c r="AH2" t="s">
+        <v>104</v>
+      </c>
+      <c r="AI2" t="s">
         <v>105</v>
       </c>
-      <c r="AI2" t="s">
+      <c r="AJ2" t="s">
         <v>106</v>
       </c>
-      <c r="AJ2" t="s">
-        <v>107</v>
-      </c>
       <c r="AN2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="AO2" t="s">
         <v>54</v>
@@ -1568,10 +1571,10 @@
         <v>54</v>
       </c>
       <c r="AZ2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="BC2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="BD2" t="s">
         <v>50</v>
@@ -1602,96 +1605,96 @@
   <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="38.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="36.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B7" s="9"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B8" s="10"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B9" s="8"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B10" s="8"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B11" s="9"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>35</v>
       </c>
@@ -1699,13 +1702,13 @@
         <v>47</v>
       </c>
       <c r="C12" t="s">
-        <v>64</v>
+        <v>128</v>
       </c>
       <c r="D12" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>36</v>
       </c>
@@ -1713,33 +1716,27 @@
         <v>62</v>
       </c>
       <c r="C13" t="s">
-        <v>65</v>
+        <v>129</v>
       </c>
       <c r="D13" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B14" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="C14" t="s">
-        <v>61</v>
-      </c>
-      <c r="D14" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>38</v>
       </c>
       <c r="B15" s="9"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>39</v>
       </c>
@@ -1747,7 +1744,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>40</v>
       </c>
@@ -1755,61 +1752,61 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>41</v>
       </c>
       <c r="B18" s="8"/>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B19" s="8"/>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B20" s="8"/>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B21" s="8"/>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B22" s="8"/>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>46</v>
       </c>
       <c r="B23" s="8"/>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>57</v>
       </c>
       <c r="B24" s="8"/>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>58</v>
       </c>
       <c r="B25" s="8"/>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>59</v>
       </c>
       <c r="B26" s="8"/>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
         <v>60</v>
       </c>

</xml_diff>